<commit_message>
Updated Iteration 3 docs
</commit_message>
<xml_diff>
--- a/docs/CS673F13P1_weeklyreport.xlsx
+++ b/docs/CS673F13P1_weeklyreport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="185">
   <si>
     <t>week #</t>
   </si>
@@ -114,6 +114,24 @@
 5- Group meeting</t>
   </si>
   <si>
+    <t>0-learning
+4-Test
+5-group meeting</t>
+  </si>
+  <si>
+    <t>4- Test the application
+5- Group meeting</t>
+  </si>
+  <si>
+    <t>11 and 12</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+4 - sytem testing and bug fixes on github.
+5 - team management
+6 - Final presentation. </t>
+  </si>
+  <si>
     <t>Wenjie Shi</t>
   </si>
   <si>
@@ -184,6 +202,22 @@
   </si>
   <si>
     <t>3 - use form helper in medicine part. 4 - test cases.</t>
+  </si>
+  <si>
+    <t>3 - medicine view use formhelper, need authentic users, use new database
+4 - modify some bugs. test medicine part.
+</t>
+  </si>
+  <si>
+    <t>3 - modify medicine bug. 4 - test medicine part, write test case.</t>
+  </si>
+  <si>
+    <t>3 - fix medicine update,delete button. use the old way to save medicine data. modify the medicine view. 
+4 - test medicine part. write test cases.
+</t>
+  </si>
+  <si>
+    <t>3 - medicine validation. 4 - test medicine part, write test case.</t>
   </si>
   <si>
     <t>Jeff Andre</t>
@@ -279,6 +313,36 @@
 6 - Presentation, SDD</t>
   </si>
   <si>
+    <t>Task Breakdown
+0 - 
+1 - reviewed web site with customer and updated requirements.
+2 - 
+3 - added medicine contraindications alert to algorithm.
+4 - Testing customer change requests.
+5 - following up on action items and team management
+6 - Project Status report</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+0 - 
+1 - reviewed web site with customer and updated requirements.
+2 - 
+3 - updated home page with customer changes. Algorithm updates and fixes.
+4 - testing bug fixes. more phpunit testing with algorithm.
+5 - team management
+6 - Updated Project Status report</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+0 - 
+1 - 
+2 - 
+3 - 
+4 - sytem testing and bug fixes on github. more phpunit testing with algorithm and bug fixes.
+5 - team management
+6 - Project presentation. Generated autodocs by phpDocumentor. SPMP and SDD updates.</t>
+  </si>
+  <si>
     <t>Jason Lu</t>
   </si>
   <si>
@@ -340,6 +404,25 @@
     <t>3 - User management</t>
   </si>
   <si>
+    <t>3 - Custom form helper
+5 - Form helper tutorial</t>
+  </si>
+  <si>
+    <t>3 -Fix bugs</t>
+  </si>
+  <si>
+    <t>3 - Fix bugs
+3 - Unit conversion JS</t>
+  </si>
+  <si>
+    <t>3 - "Remebmer me" when user sign in
+3 - User management refine</t>
+  </si>
+  <si>
+    <t>3 - Structure refactor
+3 - Fix bugs</t>
+  </si>
+  <si>
     <t>Yike Xue</t>
   </si>
   <si>
@@ -420,6 +503,41 @@
 1 - requirement analysis(update SDD)
 3 - implementation( fix some bugs)
 4 - test (test the system, try to use test tool)</t>
+  </si>
+  <si>
+    <t>0 - learning testing tool(Selenium)
+1 - requirement analysis(update SQAP and SDD  )
+4 - test (test the overall system)</t>
+  </si>
+  <si>
+    <t>0 - learning using test tool(Selenium)
+3 - implementation( fix some bugs)
+4 - test (create test cases script by Selenium)</t>
+  </si>
+  <si>
+    <t>0 - learning testing tool(Selenium)
+3 - post and fix some bugs and enhancements
+4 - test (use Selenium)</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis(update SQAP and SDD)
+3 - implementation( fix some bugs)
+4 - test (create test cases script by Selenium)
+5 - prepare for the last presentation</t>
+  </si>
+  <si>
+    <t>11,12</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis( metric statistics, update SDD and SQAP)
+3 - implementation(fix some bugs)
+4 - test(use selenium)
+5 - communication/management
+6 - prepare for the presentation
+</t>
+  </si>
+  <si>
+    <t>5 - self the peer evaluation</t>
   </si>
   <si>
     <t>Yingyuan Zhang</t>
@@ -522,9 +640,52 @@
   </si>
   <si>
     <t>0 - learning PHP
-3 - implement VisitsController's gcalgorithm()
+3 - modify visitsController's edit(), and gcalgorithm()
+3 - modify visitsController for the new requirements of customers
+3 - fix bugs at VisitsController part
+4 - testing add and show visit
+5 - attending group meeting
+6 - presentation for iteration 2</t>
+  </si>
+  <si>
+    <t>0 - learning PHP
+3 - modify visitsController for the new requirements of customers
 4 - testing visit part
 5 - attending group meeting</t>
+  </si>
+  <si>
+    <t>0 - learning PHP
+3 - add weight classification and target weight at visit part
+3 - modify visitsController for the new requirements of customers
+3 - fix bugs at visit part
+4 - testing BMI status, Target weight at visit part
+5 - attending group meeting</t>
+  </si>
+  <si>
+    <t>0 - learning PHP
+3 - modify visitsController for the new requirements of customers
+3 - fix bugs at visit part
+4 - write test cases and test BMI status and Target weight at visit part
+5 - attending group meeting</t>
+  </si>
+  <si>
+    <t>3 - modify visitsController for the new requirements of customers
+3 - fix bugs at visit part
+4 - test BMI status and Target weight at visit part
+5 - attending group meeting</t>
+  </si>
+  <si>
+    <t>3 - modify visitsController for the new requirements of customers
+3 - fix bugs at visit part
+5 - attending group meeting
+6 - prepare for final presentation</t>
+  </si>
+  <si>
+    <t>3 - modify visitsController for the new requirements of customers
+3 - fix bugs at visit part
+4 - test function in visit part
+5 - attending group meeting
+6 - prepare for final presentation</t>
   </si>
   <si>
     <t>Maura</t>
@@ -640,6 +801,50 @@
 3 - implementation (start adding plots to charts tab)
 4 - test (unit testing for ui components)
 5 - communication/management (group meetings)</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis (making sure ui matches user req'ts)
+2 - design (ui design for a1c and bmi charts)
+3 - implementation (added chart for a1c and accordian for the charts tab)
+4 - test (unit testing for ui components)
+5 - communication/management (group meetings)</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis (making sure ui matches user req'ts)
+2 - design (ui design)
+3 - implementation (implement the bmi chart, fix hover time to date conversion)
+4 - test (unit testing for ui components)
+5 - communication/management (group meetings)</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis (making sure ui matches user req'ts)
+2 - design (ui design)
+3 - implementation (finished bmi chart and refactoried some of chart and accordian code)
+4 - test (unit testing for ui components)
+5 - communication/management (group meetings)</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis (making sure ui matches user req'ts)
+2 - design (ui design)
+3 - implementation (add zooming and panning to the charts)
+4 - test (unit testing for ui components)
+5 - communication/management (group meetings)</t>
+  </si>
+  <si>
+    <t>1 - requirement analysis (making sure ui matches user req'ts)
+2 - design (ui design)
+3 - implementation (finished zooming and panning on both charts with flot.navigation, fixed hover time to date conversion bug with new moment.js library)
+4 - test (unit testing for ui components)
+5 - communication/management (group meetings)</t>
+  </si>
+  <si>
+    <t>3 - implementation (fix any ui bugs) 4 - test (unit testing for ui components)
+5 - communication/management (group meetings and prepping for final demo)</t>
+  </si>
+  <si>
+    <t>3 - implementation (finished some existing ui bugs)
+4 - test (unit testing for ui components)
+5 - communication/management (group meetings, prep for final presentation, write demo script, add details to responsible slides)</t>
   </si>
   <si>
     <t>Bogdan</t>
@@ -805,6 +1010,74 @@
 </t>
   </si>
   <si>
+    <t>Task Breakdown
+0 - learning (Selenium)
+1 - requirement analysis (customer feedback) 
+3 - implementation(chnages in view part)
+4 - test (test view pages)
+5 - communication/management (emails with the team)
+6 - unclassified (setting up Selenium, update sql scripts)</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+0 - learning ( Selenium, JUnit for PHP)
+1 - requirement analysis (customer feedback) 
+2 - design (flash messages)
+3 - implementation(flash messages)
+4 - test (test pages with Selenium and maybe wtiting tests with PHP JUnit)
+5 - communication/management (emails with the team)
+6 - unclassified (update documentation)
+</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+0 - learning ( Selenium )
+3 - implementation(flash messages)
+4 - test (testing pages with Selenium)
+5 - communication/management (emails with the team)
+6 - unclassified (update dcumentation)
+</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+0 - learning (MySQL Workbench)
+1 - requirement analysis (customer feedback) 
+2 - design (page with algorithm flowchart diagrams)
+3 - implementation(page with algorithm flowchart diagrams)
+4 - test (page with algorithm flowchart diagrams, database sript update)
+5 - communication/management (emails with the team)
+6 - unclassified (update documentation - database schema, SDD)
+</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+0 - learning (MySQL Workbench)
+1 - requirement analysis (customer feedback) 
+2 - design (page with algorithm flowchart diagrams)
+3 - implementation(page with algorithm flowchart diagrams)
+4 - test (page with algorithm flowchart diagrams, database sript)
+5 - communication/management (emails with the team)
+6 - unclassified (update documentation)
+</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+1 - requirement analysis (customer feedback) 
+4 - test (application)
+5 - communication/management (emails with the team)
+6 - unclassified (update documentation, presetation)
+</t>
+  </si>
+  <si>
+    <t>Task Breakdown
+2 - design (demo records for presentation)
+3 - implementation(text edition, fixing bugs/code improvement, sql file for demo )
+4 - test (testing patinet/visit part of application, test demo)
+5 - communication/management (emails with the team)
+6 - unclassified (update documentation, presentation preparation )
+</t>
+  </si>
+  <si>
     <t>Yulu</t>
   </si>
   <si>
@@ -844,7 +1117,8 @@
    fix the user low priority on dbproblem(4)</t>
   </si>
   <si>
-    <t>3-Add Patient Validation And medicine show page.</t>
+    <t>3-implement of Add Patient Validation 
+   medicine show page.</t>
   </si>
   <si>
     <t>0-learn js and regex rule of validation
@@ -854,6 +1128,22 @@
     <t>0-learn CakePHP form helper for the change in UI
 1-requirment analysis of Regex, rules of validation.
 3-implement. Change the validation from old version to the one on form helper based page. </t>
+  </si>
+  <si>
+    <t>1-requrment analysis of medicine validation. 
+3-implement. Make sure the Add visit page input checking work functionally.
+4-unit test of all the validation. Mainly for the problem occured in weight and height.
+</t>
+  </si>
+  <si>
+    <t>0-learn selenium
+3-fix bugs in patient and visit.
+4- unit testing</t>
+  </si>
+  <si>
+    <t>1-requirement analysis for patient and user.
+3-Try to do the secuirty testing using netsparker.
+4-unit testing for add visit</t>
   </si>
 </sst>
 </file>
@@ -1259,6 +1549,141 @@
         <v>25</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c t="s" r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c t="s" r="F8">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c t="s" r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c t="s" r="F9">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" r="A10">
+        <v>24</v>
+      </c>
+      <c t="s" r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c t="s" r="F10">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
@@ -1331,7 +1756,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -1343,7 +1768,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -1355,7 +1780,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O2">
         <v>12</v>
@@ -1366,7 +1791,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -1378,7 +1803,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F3">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -1390,7 +1815,7 @@
         <v>3</v>
       </c>
       <c t="s" r="N3">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="O3">
         <v>16</v>
@@ -1401,7 +1826,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -1413,7 +1838,7 @@
         <v>6</v>
       </c>
       <c t="s" r="F4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1428,7 +1853,7 @@
         <v>2</v>
       </c>
       <c t="s" r="N4">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="O4">
         <v>20</v>
@@ -1439,7 +1864,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -1451,7 +1876,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F5">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G5">
         <v>6</v>
@@ -1466,7 +1891,7 @@
         <v>3</v>
       </c>
       <c t="s" r="N5">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="O5">
         <v>15</v>
@@ -1477,7 +1902,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -1489,7 +1914,7 @@
         <v>3</v>
       </c>
       <c t="s" r="F6">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -1504,7 +1929,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N6">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -1515,7 +1940,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1527,7 +1952,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1536,7 +1961,7 @@
         <v>6</v>
       </c>
       <c t="s" r="N7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O7">
         <v>8</v>
@@ -1547,7 +1972,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -1559,7 +1984,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F8">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1568,7 +1993,7 @@
         <v>2</v>
       </c>
       <c t="s" r="N8">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="O8">
         <v>8</v>
@@ -1579,7 +2004,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -1591,7 +2016,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J9">
         <v>4</v>
@@ -1603,10 +2028,74 @@
         <v>2</v>
       </c>
       <c t="s" r="N9">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O9">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c t="s" r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c t="s" r="F10">
+        <v>43</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c t="s" r="N10">
+        <v>44</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>45</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c t="s" r="N11">
+        <v>46</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +2170,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1693,7 +2182,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1708,7 +2197,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="O2">
         <v>10</v>
@@ -1719,7 +2208,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>19</v>
@@ -1731,7 +2220,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F3">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1749,7 +2238,7 @@
         <v>4</v>
       </c>
       <c t="s" r="N3">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="O3">
         <v>10</v>
@@ -1760,7 +2249,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -1772,7 +2261,7 @@
         <v>5</v>
       </c>
       <c t="s" r="F4">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -1795,7 +2284,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1807,7 +2296,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F5">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1825,7 +2314,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N5">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="O5">
         <v>15</v>
@@ -1836,7 +2325,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>19</v>
@@ -1848,7 +2337,7 @@
         <v>3</v>
       </c>
       <c t="s" r="F6">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1866,7 +2355,7 @@
         <v>4</v>
       </c>
       <c t="s" r="N6">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="O6">
         <v>15</v>
@@ -1877,7 +2366,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -1889,7 +2378,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1909,7 +2398,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -1921,7 +2410,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F8">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1941,7 +2430,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>19</v>
@@ -1953,7 +2442,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -1969,6 +2458,102 @@
       </c>
       <c r="M9">
         <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c t="s" r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>15.5</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c t="s" r="F10">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>7</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>61</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>24</v>
+      </c>
+      <c t="s" r="B12">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c t="s" r="F12">
+        <v>62</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2049,7 +2634,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -2061,7 +2646,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -2085,7 +2670,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N2">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="O2">
         <v>8</v>
@@ -2096,7 +2681,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -2108,7 +2693,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F3">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -2132,7 +2717,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N3">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="O3">
         <v>12</v>
@@ -2143,7 +2728,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <f>sum(D4:E4)</f>
@@ -2157,7 +2742,7 @@
         <v>6</v>
       </c>
       <c t="s" r="F4">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -2181,7 +2766,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N4">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="O4">
         <v>6</v>
@@ -2192,7 +2777,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <f>sum(D5:E5)</f>
@@ -2206,7 +2791,7 @@
         <v>3</v>
       </c>
       <c t="s" r="F5">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -2230,7 +2815,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N5">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="O5">
         <v>6</v>
@@ -2241,7 +2826,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <f>sum(D6:E6)</f>
@@ -2255,7 +2840,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F6">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -2279,7 +2864,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N6">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="O6">
         <v>6</v>
@@ -2290,7 +2875,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <f>sum(D7:E7)</f>
@@ -2304,7 +2889,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2328,7 +2913,191 @@
         <v>0</v>
       </c>
       <c t="s" r="N7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c t="s" r="B8">
         <v>63</v>
+      </c>
+      <c r="C8">
+        <f>sum(D8:E8)</f>
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <f>sum(G8:M8)</f>
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c t="s" r="F8">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c t="s" r="N8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c t="s" r="B9">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <f>sum(D9:E9)</f>
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f>sum(G9:M9)</f>
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c t="s" r="F9">
+        <v>77</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c t="s" r="N9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c t="s" r="B10">
+        <v>63</v>
+      </c>
+      <c r="C10">
+        <f>sum(D10:E10)</f>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <f>sum(G10:M10)</f>
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c t="s" r="F10">
+        <v>78</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c t="s" r="N10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>63</v>
+      </c>
+      <c r="C11">
+        <f>sum(D11:E11)</f>
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <f>sum(G11:M11)</f>
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>79</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c t="s" r="N11">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2408,7 +3177,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -2420,7 +3189,7 @@
         <v>3</v>
       </c>
       <c t="s" r="F2">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -2432,7 +3201,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N2">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="O2">
         <v>8</v>
@@ -2443,7 +3212,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -2455,7 +3224,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F3">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -2467,7 +3236,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N3">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="O3">
         <v>8</v>
@@ -2478,7 +3247,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>9</v>
@@ -2490,7 +3259,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F4">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2502,7 +3271,7 @@
         <v>2</v>
       </c>
       <c t="s" r="N4">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="O4">
         <v>10</v>
@@ -2513,7 +3282,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -2525,7 +3294,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F5">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -2537,7 +3306,7 @@
         <v>3</v>
       </c>
       <c t="s" r="N5">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="O5">
         <v>8</v>
@@ -2548,7 +3317,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -2560,7 +3329,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F6">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="H6">
         <v>0.5</v>
@@ -2575,7 +3344,7 @@
         <v>2</v>
       </c>
       <c t="s" r="N6">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -2586,7 +3355,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -2598,7 +3367,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F7">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -2610,7 +3379,7 @@
         <v>4</v>
       </c>
       <c t="s" r="N7">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="O7">
         <v>10</v>
@@ -2621,7 +3390,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -2633,7 +3402,7 @@
         <v>1</v>
       </c>
       <c t="s" r="F8">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2645,7 +3414,7 @@
         <v>6</v>
       </c>
       <c t="s" r="N8">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="O8">
         <v>10</v>
@@ -2656,7 +3425,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -2668,7 +3437,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -2683,10 +3452,121 @@
         <v>2</v>
       </c>
       <c t="s" r="N9">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="O9">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c t="s" r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c t="s" r="F10">
+        <v>95</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c t="s" r="N10">
+        <v>96</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>97</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c t="s" r="N11">
+        <v>98</v>
+      </c>
+      <c r="O11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>99</v>
+      </c>
+      <c t="s" r="B12">
+        <v>80</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>17.5</v>
+      </c>
+      <c r="E12">
+        <v>4.5</v>
+      </c>
+      <c t="s" r="F12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>1.5</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c t="s" r="N12">
+        <v>101</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2761,7 +3641,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -2773,7 +3653,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -2797,7 +3677,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N2">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="O2">
         <v>12</v>
@@ -2808,7 +3688,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -2820,7 +3700,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F3">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="G3">
         <v>4.5</v>
@@ -2844,7 +3724,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N3">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="O3">
         <v>12</v>
@@ -2855,7 +3735,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>14.5</v>
@@ -2867,7 +3747,7 @@
         <v>6</v>
       </c>
       <c t="s" r="F4">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="G4">
         <v>5.5</v>
@@ -2891,7 +3771,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N4">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="O4">
         <v>14</v>
@@ -2902,7 +3782,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>13</v>
@@ -2914,7 +3794,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F5">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -2938,7 +3818,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N5">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="O5">
         <v>14</v>
@@ -2949,19 +3829,19 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
         <v>15</v>
       </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c t="s" r="F6">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="G6">
         <v>3.5</v>
@@ -2973,7 +3853,7 @@
         <v>0.5</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2985,7 +3865,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N6">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="O6">
         <v>15</v>
@@ -2996,19 +3876,19 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
         <v>16</v>
       </c>
-      <c r="D7">
-        <v>14</v>
-      </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -3020,7 +3900,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3032,7 +3912,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N7">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="O7">
         <v>13</v>
@@ -3043,7 +3923,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -3055,7 +3935,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F8">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3079,7 +3959,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N8">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="O8">
         <v>14</v>
@@ -3090,19 +3970,19 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3114,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -3123,13 +4003,148 @@
         <v>2</v>
       </c>
       <c r="M9">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c t="s" r="N9">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="O9">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c t="s" r="B10">
+        <v>102</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>13.5</v>
+      </c>
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c t="s" r="F10">
+        <v>119</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>1.5</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c t="s" r="N10">
+        <v>120</v>
+      </c>
+      <c r="O10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>102</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>121</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c t="s" r="N11">
+        <v>122</v>
+      </c>
+      <c r="O11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>24</v>
+      </c>
+      <c t="s" r="B12">
+        <v>102</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c t="s" r="F12">
+        <v>123</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3206,7 +4221,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3218,7 +4233,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -3242,7 +4257,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N2">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="O2">
         <v>10</v>
@@ -3253,7 +4268,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3265,7 +4280,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F3">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -3286,7 +4301,7 @@
         <v>0.5</v>
       </c>
       <c t="s" r="N3">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="O3">
         <v>12</v>
@@ -3297,7 +4312,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -3309,7 +4324,7 @@
         <v>3</v>
       </c>
       <c t="s" r="F4">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -3324,7 +4339,7 @@
         <v>3</v>
       </c>
       <c t="s" r="N4">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="O4">
         <v>15</v>
@@ -3335,7 +4350,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -3347,7 +4362,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F5">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -3362,7 +4377,7 @@
         <v>4</v>
       </c>
       <c t="s" r="N5">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="O5">
         <v>16</v>
@@ -3373,7 +4388,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C6">
         <v>20.5</v>
@@ -3385,7 +4400,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F6">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3409,7 +4424,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N6">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="O6">
         <v>15</v>
@@ -3420,7 +4435,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -3432,7 +4447,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3456,7 +4471,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N7">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="O7">
         <v>12</v>
@@ -3467,7 +4482,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3479,7 +4494,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F8">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -3500,7 +4515,7 @@
         <v>2</v>
       </c>
       <c t="s" r="N8">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="O8">
         <v>15</v>
@@ -3511,7 +4526,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C9">
         <v>21</v>
@@ -3523,7 +4538,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3544,7 +4559,7 @@
         <v>2</v>
       </c>
       <c t="s" r="N9">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="O9">
         <v>10</v>
@@ -3555,7 +4570,169 @@
         <v>9</v>
       </c>
       <c t="s" r="B10">
-        <v>95</v>
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c t="s" r="F10">
+        <v>141</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>7.5</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c t="s" r="N10">
+        <v>142</v>
+      </c>
+      <c r="O10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>124</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>143</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>0.5</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c t="s" r="N11">
+        <v>144</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c t="s" r="B12">
+        <v>124</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c t="s" r="F12">
+        <v>145</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c t="s" r="N12">
+        <v>146</v>
+      </c>
+      <c r="O12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c t="s" r="B13">
+        <v>124</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c t="s" r="F13">
+        <v>147</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3631,7 +4808,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3643,7 +4820,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="G2">
         <v>0.5</v>
@@ -3667,7 +4844,7 @@
         <v>3</v>
       </c>
       <c t="s" r="N2">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="O2">
         <v>12</v>
@@ -3678,7 +4855,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C3">
         <v>15.5</v>
@@ -3690,7 +4867,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F3">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3714,7 +4891,7 @@
         <v>4</v>
       </c>
       <c t="s" r="N3">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="O3">
         <v>15</v>
@@ -3725,7 +4902,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C4">
         <v>19</v>
@@ -3737,7 +4914,7 @@
         <v>5</v>
       </c>
       <c t="s" r="F4">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -3761,7 +4938,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N4">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="O4">
         <v>15</v>
@@ -3772,7 +4949,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C5">
         <v>19</v>
@@ -3784,7 +4961,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F5">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -3808,7 +4985,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N5">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="O5">
         <v>15</v>
@@ -3819,7 +4996,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>7.5</v>
@@ -3831,7 +5008,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F6">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -3855,7 +5032,7 @@
         <v>0.5</v>
       </c>
       <c t="s" r="N6">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="O6">
         <v>15</v>
@@ -3866,7 +5043,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C7">
         <v>11.5</v>
@@ -3878,7 +5055,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -3902,7 +5079,7 @@
         <v>0.5</v>
       </c>
       <c t="s" r="N7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="O7">
         <v>15</v>
@@ -3913,7 +5090,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3925,7 +5102,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F8">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="G8">
         <v>1.5</v>
@@ -3949,7 +5126,7 @@
         <v>0</v>
       </c>
       <c t="s" r="N8">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="O8">
         <v>15</v>
@@ -3960,7 +5137,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C9">
         <v>13.25</v>
@@ -3972,7 +5149,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3996,7 +5173,7 @@
         <v>3</v>
       </c>
       <c t="s" r="N9">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="O9">
         <v>15</v>
@@ -4007,7 +5184,181 @@
         <v>9</v>
       </c>
       <c t="s" r="B10">
-        <v>112</v>
+        <v>148</v>
+      </c>
+      <c r="C10">
+        <v>10.25</v>
+      </c>
+      <c r="D10">
+        <v>11.75</v>
+      </c>
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c t="s" r="F10">
+        <v>165</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0.25</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c t="s" r="N10">
+        <v>166</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>148</v>
+      </c>
+      <c r="C11">
+        <v>7.5</v>
+      </c>
+      <c r="D11">
+        <v>9.5</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>167</v>
+      </c>
+      <c r="G11">
+        <v>1.5</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c t="s" r="N11">
+        <v>168</v>
+      </c>
+      <c r="O11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c t="s" r="B12">
+        <v>148</v>
+      </c>
+      <c r="C12">
+        <v>10.5</v>
+      </c>
+      <c r="D12">
+        <v>12.5</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c t="s" r="F12">
+        <v>169</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c t="s" r="N12">
+        <v>170</v>
+      </c>
+      <c r="O12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c t="s" r="B13">
+        <v>148</v>
+      </c>
+      <c r="C13">
+        <v>9.5</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>4.5</v>
+      </c>
+      <c t="s" r="F13">
+        <v>171</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.5</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4082,7 +5433,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B2">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -4094,7 +5445,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F2">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -4120,7 +5471,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B3">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -4132,7 +5483,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F3">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -4147,7 +5498,7 @@
         <v>1</v>
       </c>
       <c t="s" r="N3">
-        <v>132</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4">
@@ -4155,7 +5506,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B4">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C4">
         <v>13</v>
@@ -4167,7 +5518,7 @@
         <v>5</v>
       </c>
       <c t="s" r="F4">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -4187,7 +5538,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B5">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C5">
         <v>17</v>
@@ -4199,7 +5550,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F5">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -4213,7 +5564,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B6">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C6">
         <v>21</v>
@@ -4225,7 +5576,7 @@
         <v>4</v>
       </c>
       <c t="s" r="F6">
-        <v>135</v>
+        <v>178</v>
       </c>
       <c r="J6">
         <v>13</v>
@@ -4239,7 +5590,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -4251,7 +5602,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="J7">
         <v>8</v>
@@ -4265,7 +5616,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -4277,7 +5628,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F8">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -4291,7 +5642,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B9">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -4303,7 +5654,7 @@
         <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -4313,6 +5664,93 @@
       </c>
       <c r="J9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c t="s" r="B10">
+        <v>172</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c t="s" r="F10">
+        <v>182</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="J10">
+        <v>8.5</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c t="s" r="B11">
+        <v>172</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c t="s" r="F11">
+        <v>183</v>
+      </c>
+      <c r="G11">
+        <v>1.5</v>
+      </c>
+      <c r="J11">
+        <v>2.5</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>24</v>
+      </c>
+      <c t="s" r="B12">
+        <v>172</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c t="s" r="F12">
+        <v>184</v>
+      </c>
+      <c r="H12">
+        <v>1.5</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>